<commit_message>
[excel-pipeline] hash_id:995ab6d commit_msg:增加单位初始行动条位置 ...
</commit_message>
<xml_diff>
--- a/config/excel/DemoStage.xlsx
+++ b/config/excel/DemoStage.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dd\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EastEden\excel\global\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33308B04-59ED-4523-A4D2-2D62100C46D8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A388B7E-DCFA-4157-9C42-B89163DFB1E5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DemoStage" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -35,10 +35,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>y</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>战斗单位</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -83,14 +79,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>横坐标</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>纵坐标</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>camp</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -108,6 +96,34 @@
   </si>
   <si>
     <t>属性ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初始行动条</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>initialCom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>坐标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>坐标-x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>坐标-z</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -397,7 +413,7 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
@@ -407,8 +423,12 @@
         <right style="thin">
           <color theme="1"/>
         </right>
-        <top/>
-        <bottom/>
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
         <vertical style="thin">
           <color theme="1"/>
         </vertical>
@@ -536,13 +556,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color theme="1"/>
@@ -560,6 +573,32 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color theme="1"/>
+        </left>
+        <right style="thin">
+          <color theme="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color theme="1"/>
+        </vertical>
+        <horizontal style="thin">
+          <color theme="1"/>
+        </horizontal>
+      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -575,14 +614,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F3E60E7D-9F12-4EEF-B2F0-23523298C422}" name="表3" displayName="表3" ref="C1:G14" totalsRowShown="0" headerRowDxfId="0" dataDxfId="9" headerRowBorderDxfId="7" tableBorderDxfId="8" totalsRowBorderDxfId="6">
-  <autoFilter ref="C1:G14" xr:uid="{45878729-301F-4F1A-811A-48E769BE0429}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F3E60E7D-9F12-4EEF-B2F0-23523298C422}" name="表3" displayName="表3" ref="C1:H14" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+  <autoFilter ref="C1:H14" xr:uid="{45878729-301F-4F1A-811A-48E769BE0429}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{6EAB8209-2CF2-42D2-A245-A28B42BF718D}" name="战斗单位" dataDxfId="5"/>
     <tableColumn id="2" xr3:uid="{73F6F32E-161D-40CC-A46A-0C25F0B2B558}" name="友军/敌军" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{46317446-A639-40F9-93A1-12FC3AA6E63C}" name="横坐标" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{AEA7658E-CD43-4E9F-B589-3001FB0F44B3}" name="纵坐标" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{46317446-A639-40F9-93A1-12FC3AA6E63C}" name="坐标-x" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{AEA7658E-CD43-4E9F-B589-3001FB0F44B3}" name="坐标-z" dataDxfId="2"/>
     <tableColumn id="5" xr3:uid="{04D0A89A-03DA-4671-ABD7-6B87749657EC}" name="属性ID" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{16A3B66C-9203-4A32-A586-966C65299508}" name="初始行动条" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -851,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24467693-45A3-4494-81BE-A1051D46A014}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -862,120 +902,136 @@
     <col min="1" max="2" width="9" style="1"/>
     <col min="3" max="3" width="10.25" style="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="1"/>
+    <col min="5" max="7" width="9" style="1"/>
+    <col min="8" max="8" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>8</v>
-      </c>
       <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H1" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="4"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
       <c r="B2" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="16"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H2" s="9"/>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>1</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="H4" s="4"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="5" t="s">
-        <v>12</v>
       </c>
       <c r="C5" s="11"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
       <c r="G5" s="13"/>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H5" s="12"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="4"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B7" s="5"/>
       <c r="C7" s="14">
         <v>1</v>
@@ -992,9 +1048,12 @@
       <c r="G7" s="16">
         <v>1</v>
       </c>
-      <c r="H7" s="4"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H7" s="15">
+        <v>0.1</v>
+      </c>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B8" s="5"/>
       <c r="C8" s="14">
         <v>2</v>
@@ -1011,9 +1070,12 @@
       <c r="G8" s="16">
         <v>2</v>
       </c>
-      <c r="H8" s="4"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H8" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B9" s="5"/>
       <c r="C9" s="14">
         <v>3</v>
@@ -1030,9 +1092,12 @@
       <c r="G9" s="16">
         <v>3</v>
       </c>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H9" s="15">
+        <v>0.35</v>
+      </c>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B10" s="5"/>
       <c r="C10" s="14">
         <v>4</v>
@@ -1049,9 +1114,12 @@
       <c r="G10" s="16">
         <v>4</v>
       </c>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H10" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" s="5"/>
       <c r="C11" s="14">
         <v>5</v>
@@ -1068,9 +1136,12 @@
       <c r="G11" s="16">
         <v>5</v>
       </c>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H11" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
       <c r="C12" s="14">
         <v>6</v>
@@ -1087,9 +1158,12 @@
       <c r="G12" s="16">
         <v>5</v>
       </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H12" s="15">
+        <v>0.6</v>
+      </c>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="C13" s="14">
         <v>7</v>
@@ -1106,9 +1180,12 @@
       <c r="G13" s="16">
         <v>6</v>
       </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H13" s="15">
+        <v>0.45</v>
+      </c>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
       <c r="C14" s="17">
         <v>8</v>
@@ -1125,14 +1202,18 @@
       <c r="G14" s="19">
         <v>7</v>
       </c>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H14" s="18">
+        <v>0</v>
+      </c>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>